<commit_message>
Add fields to the syntax tree design of some nodes.
</commit_message>
<xml_diff>
--- a/SyntaxTreeDesign.xlsx
+++ b/SyntaxTreeDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvador/Desktop/Interpreter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2264F1FE-B960-6949-B618-9EF65719D2B5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0908D952-6D87-544C-A108-8B31247C3878}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="2420" windowWidth="28040" windowHeight="17440" xr2:uid="{5BBD8E83-C19B-DE45-A66B-485CC8C5C80F}"/>
+    <workbookView xWindow="11700" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{5BBD8E83-C19B-DE45-A66B-485CC8C5C80F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Syntax Tree Node</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>print</t>
+  </si>
+  <si>
+    <t>instruction</t>
+  </si>
+  <si>
+    <t>expr</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -415,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B070D2-1826-DA46-AB62-B65509CC00BF}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,10 +454,25 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finish the design of the syntax tree.
</commit_message>
<xml_diff>
--- a/SyntaxTreeDesign.xlsx
+++ b/SyntaxTreeDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvador/Desktop/Interpreter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0908D952-6D87-544C-A108-8B31247C3878}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21B51B3-7452-1D4D-B772-D66C6DC7A2CD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{5BBD8E83-C19B-DE45-A66B-485CC8C5C80F}"/>
+    <workbookView xWindow="2060" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{5BBD8E83-C19B-DE45-A66B-485CC8C5C80F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
   <si>
     <t>Syntax Tree Node</t>
   </si>
@@ -45,24 +45,134 @@
     <t>print</t>
   </si>
   <si>
-    <t>instruction</t>
-  </si>
-  <si>
-    <t>expr</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
+    <t>if</t>
+  </si>
+  <si>
+    <t>ifelse</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>numi</t>
+  </si>
+  <si>
+    <t>numf</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>ptr (id, value or operator)</t>
+  </si>
+  <si>
+    <t>condition (ptr to comparison operator)</t>
+  </si>
+  <si>
+    <t>ptr to stmt</t>
+  </si>
+  <si>
+    <t>ptr to if stmt</t>
+  </si>
+  <si>
+    <t>ptr to else stmt</t>
+  </si>
+  <si>
+    <t>ptr to set</t>
+  </si>
+  <si>
+    <t>to_expression</t>
+  </si>
+  <si>
+    <t>step_expression</t>
+  </si>
+  <si>
+    <t>stmt</t>
+  </si>
+  <si>
+    <t>ptr to symbol</t>
+  </si>
+  <si>
+    <t>pointer to next tree node</t>
+  </si>
+  <si>
+    <t>ptr to id</t>
+  </si>
+  <si>
+    <t>ptr to instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>node type</t>
+  </si>
+  <si>
+    <t>node name</t>
+  </si>
+  <si>
+    <t>ptr1</t>
+  </si>
+  <si>
+    <t>ptr2</t>
+  </si>
+  <si>
+    <t>ptr3</t>
+  </si>
+  <si>
+    <t>ptr4</t>
+  </si>
+  <si>
+    <t>ptr5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -101,14 +211,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -425,69 +585,526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B070D2-1826-DA46-AB62-B65509CC00BF}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add the definition of the syntax tree node.
</commit_message>
<xml_diff>
--- a/SyntaxTreeDesign.xlsx
+++ b/SyntaxTreeDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvador/Desktop/Interpreter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21B51B3-7452-1D4D-B772-D66C6DC7A2CD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A125CC94-38DF-F949-B68E-16F52D67710E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{5BBD8E83-C19B-DE45-A66B-485CC8C5C80F}"/>
   </bookViews>
@@ -156,7 +156,7 @@
     <t>ptr4</t>
   </si>
   <si>
-    <t>ptr5</t>
+    <t>next ptr</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -244,8 +244,36 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -255,20 +283,20 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -588,7 +616,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,55 +633,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">

</xml_diff>

<commit_message>
Add fields to the 'SymbolTableNode' definition for supporting functions. Add the PDF file with the last homework description.
</commit_message>
<xml_diff>
--- a/SyntaxTreeDesign.xlsx
+++ b/SyntaxTreeDesign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvador/Desktop/Interpreter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A125CC94-38DF-F949-B68E-16F52D67710E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B93B39-5515-8645-A9F9-59BDA3548470}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{5BBD8E83-C19B-DE45-A66B-485CC8C5C80F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>Syntax Tree Node</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>next ptr</t>
+  </si>
+  <si>
+    <t>function</t>
   </si>
 </sst>
 </file>
@@ -280,11 +283,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -294,11 +302,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B070D2-1826-DA46-AB62-B65509CC00BF}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,41 +640,41 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1129,6 +1133,23 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="10">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>